<commit_message>
Update max_length parameters in page_chunks.json and products.json to optimize data handling
</commit_message>
<xml_diff>
--- a/Management/Costes.xlsx
+++ b/Management/Costes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schem\Dropbox\git_projects\Addictive_POC\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{C84AB3E8-47FE-409F-AF93-F299DF8BBA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8631A86D-DCE8-4B30-AF8E-E87ABE4AD90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{6F0A77F9-F3DF-40B3-B21A-6AC7A82C1C5A}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Hosting</t>
   </si>
@@ -115,6 +114,9 @@
   </si>
   <si>
     <t>https://groq.com/pricing</t>
+  </si>
+  <si>
+    <t>Hosting + backup diario</t>
   </si>
 </sst>
 </file>
@@ -541,12 +543,12 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.265625" customWidth="1"/>
     <col min="3" max="3" width="30.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="16.3984375" customWidth="1"/>
@@ -615,7 +617,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -624,72 +626,82 @@
         <v>8</v>
       </c>
       <c r="D3" s="3">
-        <v>0.35</v>
+        <v>928.37</v>
       </c>
       <c r="E3" s="4">
         <v>0.21</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="5">
         <f>D3*(1+E3)</f>
-        <v>0.42349999999999999</v>
+        <v>1123.3277</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="H3" s="3">
-        <f>F3</f>
-        <v>0.42349999999999999</v>
+        <f>F3/24</f>
+        <v>46.805320833333333</v>
       </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.35</v>
       </c>
       <c r="E4" s="4">
         <v>0.21</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <f>D4*(1+E4)</f>
-        <v>7.26</v>
+        <v>0.42349999999999999</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5">
-        <f>F4/6</f>
-        <v>1.21</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H4" s="3">
+        <f>F4</f>
+        <v>0.42349999999999999</v>
+      </c>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D5" s="5">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="F5" s="5">
+        <f>D5*(1+E5)</f>
+        <v>7.26</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="5">
+        <f>F5/6</f>
+        <v>1.21</v>
+      </c>
       <c r="I5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -697,10 +709,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -712,15 +724,23 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
@@ -824,10 +844,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{121FBD3D-231E-4ED6-B81C-EE6BAC7CF949}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{DCDCFA2D-3305-4D37-997E-B1F628287798}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{D7F2595C-3913-4347-ABC7-EF9ED1DF779D}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{AA8EA795-9403-4BF2-8699-1DE3B8DB2473}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{3BEA2669-2A49-4BBB-9C41-86CED72E640B}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{DCDCFA2D-3305-4D37-997E-B1F628287798}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{D7F2595C-3913-4347-ABC7-EF9ED1DF779D}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{AA8EA795-9403-4BF2-8699-1DE3B8DB2473}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{3BEA2669-2A49-4BBB-9C41-86CED72E640B}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{38DDBF9C-D579-443F-820F-50A766466DA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>